<commit_message>
Update DRC to remove reference to EV charging
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -18,7 +18,7 @@
     <sheet name="DRC-BDRC" sheetId="5" r:id="rId4"/>
     <sheet name="DRC-PADRC" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>Year</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t xml:space="preserve">That was scaled for future BAU projections as per the growth in peak demand output of EPS. </t>
+  </si>
+  <si>
+    <t>However, we adjust to remove the contribution from EV charging, which</t>
+  </si>
+  <si>
+    <t>is calculated separately in the EPS.</t>
   </si>
 </sst>
 </file>
@@ -776,13 +782,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>481086</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>62372</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1257,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1483,6 +1489,7 @@
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
     <hyperlink ref="B22" r:id="rId2"/>
+    <hyperlink ref="G8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
@@ -1496,10 +1503,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1546,7 +1553,8 @@
         <v>40</v>
       </c>
       <c r="J2" s="53">
-        <v>90</v>
+        <f>90-12.5</f>
+        <v>77.5</v>
       </c>
       <c r="K2" s="53">
         <v>180</v>
@@ -1561,7 +1569,8 @@
         <v>922.18845458994383</v>
       </c>
       <c r="C3">
-        <v>90000</v>
+        <f>J2*1000</f>
+        <v>77500</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.45">
@@ -1574,311 +1583,324 @@
         <v>84</v>
       </c>
     </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="G6" s="51" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7">
-        <v>2019</v>
-      </c>
-      <c r="C7">
-        <v>2020</v>
-      </c>
-      <c r="D7">
-        <v>2021</v>
-      </c>
-      <c r="E7">
-        <v>2022</v>
-      </c>
-      <c r="F7">
-        <v>2023</v>
-      </c>
-      <c r="G7">
-        <v>2024</v>
-      </c>
-      <c r="H7">
-        <v>2025</v>
-      </c>
-      <c r="I7">
-        <v>2026</v>
-      </c>
-      <c r="J7">
-        <v>2027</v>
-      </c>
-      <c r="K7">
-        <v>2028</v>
-      </c>
-      <c r="L7">
-        <v>2029</v>
-      </c>
-      <c r="M7">
-        <v>2030</v>
-      </c>
-      <c r="N7">
-        <v>2031</v>
-      </c>
-      <c r="O7">
-        <v>2032</v>
-      </c>
-      <c r="P7">
-        <v>2033</v>
-      </c>
-      <c r="Q7">
-        <v>2034</v>
-      </c>
-      <c r="R7">
-        <v>2035</v>
-      </c>
-      <c r="S7">
-        <v>2036</v>
-      </c>
-      <c r="T7">
-        <v>2037</v>
-      </c>
-      <c r="U7">
-        <v>2038</v>
-      </c>
-      <c r="V7">
-        <v>2039</v>
-      </c>
-      <c r="W7">
-        <v>2040</v>
-      </c>
-      <c r="X7">
-        <v>2041</v>
-      </c>
-      <c r="Y7">
-        <v>2042</v>
-      </c>
-      <c r="Z7">
-        <v>2043</v>
-      </c>
-      <c r="AA7">
-        <v>2044</v>
-      </c>
-      <c r="AB7">
-        <v>2045</v>
-      </c>
-      <c r="AC7">
-        <v>2046</v>
-      </c>
-      <c r="AD7">
-        <v>2047</v>
-      </c>
-      <c r="AE7">
-        <v>2048</v>
-      </c>
-      <c r="AF7">
-        <v>2049</v>
-      </c>
-      <c r="AG7">
-        <v>2050</v>
+      <c r="G7" s="51" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8">
-        <v>262201</v>
-      </c>
-      <c r="C8">
-        <v>266686</v>
-      </c>
-      <c r="D8">
-        <v>284656</v>
-      </c>
-      <c r="E8">
-        <v>301356</v>
-      </c>
-      <c r="F8">
-        <v>320951</v>
-      </c>
-      <c r="G8">
-        <v>335265</v>
-      </c>
-      <c r="H8">
-        <v>348114</v>
-      </c>
-      <c r="I8">
-        <v>359564</v>
-      </c>
-      <c r="J8">
-        <v>370152</v>
-      </c>
-      <c r="K8">
-        <v>386031</v>
-      </c>
-      <c r="L8">
-        <v>400290</v>
-      </c>
-      <c r="M8">
-        <v>412327</v>
-      </c>
-      <c r="N8">
-        <v>430699</v>
-      </c>
-      <c r="O8">
-        <v>446727</v>
-      </c>
-      <c r="P8">
-        <v>463696</v>
-      </c>
-      <c r="Q8">
-        <v>478596</v>
-      </c>
-      <c r="R8">
-        <v>492010</v>
-      </c>
-      <c r="S8">
-        <v>503064</v>
-      </c>
-      <c r="T8">
-        <v>514062</v>
-      </c>
-      <c r="U8">
-        <v>523941</v>
-      </c>
-      <c r="V8">
-        <v>532239</v>
-      </c>
-      <c r="W8">
-        <v>536631</v>
-      </c>
-      <c r="X8">
-        <v>537666</v>
-      </c>
-      <c r="Y8">
-        <v>536933</v>
-      </c>
-      <c r="Z8">
-        <v>526591</v>
-      </c>
-      <c r="AA8">
-        <v>515628</v>
-      </c>
-      <c r="AB8">
-        <v>502008</v>
-      </c>
-      <c r="AC8">
-        <v>480978</v>
-      </c>
-      <c r="AD8">
-        <v>462694</v>
-      </c>
-      <c r="AE8">
-        <v>437808</v>
-      </c>
-      <c r="AF8">
-        <v>410966</v>
-      </c>
-      <c r="AG8">
-        <v>380395</v>
-      </c>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>2019</v>
+      </c>
+      <c r="C9">
+        <v>2020</v>
+      </c>
+      <c r="D9">
+        <v>2021</v>
+      </c>
+      <c r="E9">
+        <v>2022</v>
+      </c>
+      <c r="F9">
+        <v>2023</v>
+      </c>
+      <c r="G9">
+        <v>2024</v>
+      </c>
+      <c r="H9">
+        <v>2025</v>
+      </c>
+      <c r="I9">
+        <v>2026</v>
+      </c>
+      <c r="J9">
+        <v>2027</v>
+      </c>
+      <c r="K9">
+        <v>2028</v>
+      </c>
+      <c r="L9">
+        <v>2029</v>
+      </c>
+      <c r="M9">
+        <v>2030</v>
+      </c>
+      <c r="N9">
+        <v>2031</v>
+      </c>
+      <c r="O9">
+        <v>2032</v>
+      </c>
+      <c r="P9">
+        <v>2033</v>
+      </c>
+      <c r="Q9">
+        <v>2034</v>
+      </c>
+      <c r="R9">
+        <v>2035</v>
+      </c>
+      <c r="S9">
+        <v>2036</v>
+      </c>
+      <c r="T9">
+        <v>2037</v>
+      </c>
+      <c r="U9">
+        <v>2038</v>
+      </c>
+      <c r="V9">
+        <v>2039</v>
+      </c>
+      <c r="W9">
+        <v>2040</v>
+      </c>
+      <c r="X9">
+        <v>2041</v>
+      </c>
+      <c r="Y9">
+        <v>2042</v>
+      </c>
+      <c r="Z9">
+        <v>2043</v>
+      </c>
+      <c r="AA9">
+        <v>2044</v>
+      </c>
+      <c r="AB9">
+        <v>2045</v>
+      </c>
+      <c r="AC9">
+        <v>2046</v>
+      </c>
+      <c r="AD9">
+        <v>2047</v>
+      </c>
+      <c r="AE9">
+        <v>2048</v>
+      </c>
+      <c r="AF9">
+        <v>2049</v>
+      </c>
+      <c r="AG9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>262201</v>
+      </c>
+      <c r="C10">
+        <v>266686</v>
+      </c>
+      <c r="D10">
+        <v>284656</v>
+      </c>
+      <c r="E10">
+        <v>301356</v>
+      </c>
+      <c r="F10">
+        <v>320951</v>
+      </c>
+      <c r="G10">
+        <v>335265</v>
+      </c>
+      <c r="H10">
+        <v>348114</v>
+      </c>
+      <c r="I10">
+        <v>359564</v>
+      </c>
+      <c r="J10">
+        <v>370152</v>
+      </c>
+      <c r="K10">
+        <v>386031</v>
+      </c>
+      <c r="L10">
+        <v>400290</v>
+      </c>
+      <c r="M10">
+        <v>412327</v>
+      </c>
+      <c r="N10">
+        <v>430699</v>
+      </c>
+      <c r="O10">
+        <v>446727</v>
+      </c>
+      <c r="P10">
+        <v>463696</v>
+      </c>
+      <c r="Q10">
+        <v>478596</v>
+      </c>
+      <c r="R10">
+        <v>492010</v>
+      </c>
+      <c r="S10">
+        <v>503064</v>
+      </c>
+      <c r="T10">
+        <v>514062</v>
+      </c>
+      <c r="U10">
+        <v>523941</v>
+      </c>
+      <c r="V10">
+        <v>532239</v>
+      </c>
+      <c r="W10">
+        <v>536631</v>
+      </c>
+      <c r="X10">
+        <v>537666</v>
+      </c>
+      <c r="Y10">
+        <v>536933</v>
+      </c>
+      <c r="Z10">
+        <v>526591</v>
+      </c>
+      <c r="AA10">
+        <v>515628</v>
+      </c>
+      <c r="AB10">
+        <v>502008</v>
+      </c>
+      <c r="AC10">
+        <v>480978</v>
+      </c>
+      <c r="AD10">
+        <v>462694</v>
+      </c>
+      <c r="AE10">
+        <v>437808</v>
+      </c>
+      <c r="AF10">
+        <v>410966</v>
+      </c>
+      <c r="AG10">
+        <v>380395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>173800</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>171183</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>179976</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <v>190340</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>200057</v>
       </c>
-      <c r="G9">
+      <c r="G11">
         <v>207445</v>
       </c>
-      <c r="H9">
+      <c r="H11">
         <v>214344</v>
       </c>
-      <c r="I9">
+      <c r="I11">
         <v>220464</v>
       </c>
-      <c r="J9">
+      <c r="J11">
         <v>226506</v>
       </c>
-      <c r="K9">
+      <c r="K11">
         <v>230307</v>
       </c>
-      <c r="L9">
+      <c r="L11">
         <v>233659</v>
       </c>
-      <c r="M9">
+      <c r="M11">
         <v>235732</v>
       </c>
-      <c r="N9">
+      <c r="N11">
         <v>244440</v>
       </c>
-      <c r="O9">
+      <c r="O11">
         <v>253558</v>
       </c>
-      <c r="P9">
+      <c r="P11">
         <v>261443</v>
       </c>
-      <c r="Q9">
+      <c r="Q11">
         <v>268575</v>
       </c>
-      <c r="R9">
+      <c r="R11">
         <v>275152</v>
       </c>
-      <c r="S9">
+      <c r="S11">
         <v>281129</v>
       </c>
-      <c r="T9">
+      <c r="T11">
         <v>286490</v>
       </c>
-      <c r="U9">
+      <c r="U11">
         <v>292265</v>
       </c>
-      <c r="V9">
+      <c r="V11">
         <v>297605</v>
       </c>
-      <c r="W9">
+      <c r="W11">
         <v>300694</v>
       </c>
-      <c r="X9">
+      <c r="X11">
         <v>301757</v>
       </c>
-      <c r="Y9">
+      <c r="Y11">
         <v>302059</v>
       </c>
-      <c r="Z9">
+      <c r="Z11">
         <v>297336</v>
       </c>
-      <c r="AA9">
+      <c r="AA11">
         <v>290606</v>
       </c>
-      <c r="AB9">
+      <c r="AB11">
         <v>283666</v>
       </c>
-      <c r="AC9">
+      <c r="AC11">
         <v>273523</v>
       </c>
-      <c r="AD9">
+      <c r="AD11">
         <v>263033</v>
       </c>
-      <c r="AE9">
+      <c r="AE11">
         <v>250773</v>
       </c>
-      <c r="AF9">
+      <c r="AF11">
         <v>236428</v>
       </c>
-      <c r="AG9">
+      <c r="AG11">
         <v>220010</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G27" s="51" t="s">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G29" s="51" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2931,8 +2953,8 @@
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3080,127 +3102,127 @@
         <v>922.18845458994383</v>
       </c>
       <c r="G2" s="9">
-        <f>$F$2*('Revised Calcs_India'!C8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!C10/'Revised Calcs_India'!$B$10)</f>
         <v>937.96267062587003</v>
       </c>
       <c r="H2" s="9">
-        <f>$F$2*('Revised Calcs_India'!D8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!D10/'Revised Calcs_India'!$B$10)</f>
         <v>1001.1650479203171</v>
       </c>
       <c r="I2" s="9">
-        <f>$F$2*('Revised Calcs_India'!E8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!E10/'Revised Calcs_India'!$B$10)</f>
         <v>1059.9007018333534</v>
       </c>
       <c r="J2" s="9">
-        <f>$F$2*('Revised Calcs_India'!F8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!F10/'Revised Calcs_India'!$B$10)</f>
         <v>1128.8183747929911</v>
       </c>
       <c r="K2" s="9">
-        <f>$F$2*('Revised Calcs_India'!G8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!G10/'Revised Calcs_India'!$B$10)</f>
         <v>1179.1622161170153</v>
       </c>
       <c r="L2" s="9">
-        <f>$F$2*('Revised Calcs_India'!H8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!H10/'Revised Calcs_India'!$B$10)</f>
         <v>1224.353498579806</v>
       </c>
       <c r="M2" s="9">
-        <f>$F$2*('Revised Calcs_India'!I8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!I10/'Revised Calcs_India'!$B$10)</f>
         <v>1264.6243511129956</v>
       </c>
       <c r="N2" s="9">
-        <f>$F$2*('Revised Calcs_India'!J8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!J10/'Revised Calcs_India'!$B$10)</f>
         <v>1301.8634591148657</v>
       </c>
       <c r="O2" s="9">
-        <f>$F$2*('Revised Calcs_India'!K8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!K10/'Revised Calcs_India'!$B$10)</f>
         <v>1357.7115698025964</v>
       </c>
       <c r="P2" s="9">
-        <f>$F$2*('Revised Calcs_India'!L8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!L10/'Revised Calcs_India'!$B$10)</f>
         <v>1407.8619703502604</v>
       </c>
       <c r="Q2" s="9">
-        <f>$F$2*('Revised Calcs_India'!M8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!M10/'Revised Calcs_India'!$B$10)</f>
         <v>1450.1973635329682</v>
       </c>
       <c r="R2" s="9">
-        <f>$F$2*('Revised Calcs_India'!N8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!N10/'Revised Calcs_India'!$B$10)</f>
         <v>1514.8136170473576</v>
       </c>
       <c r="S2" s="9">
-        <f>$F$2*('Revised Calcs_India'!O8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!O10/'Revised Calcs_India'!$B$10)</f>
         <v>1571.1857763837736</v>
       </c>
       <c r="T2" s="9">
-        <f>$F$2*('Revised Calcs_India'!P8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!P10/'Revised Calcs_India'!$B$10)</f>
         <v>1630.8675315484631</v>
       </c>
       <c r="U2" s="9">
-        <f>$F$2*('Revised Calcs_India'!Q8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!Q10/'Revised Calcs_India'!$B$10)</f>
         <v>1683.2723964169807</v>
       </c>
       <c r="V2" s="9">
-        <f>$F$2*('Revised Calcs_India'!R8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!R10/'Revised Calcs_India'!$B$10)</f>
         <v>1730.4508432187454</v>
       </c>
       <c r="W2" s="9">
-        <f>$F$2*('Revised Calcs_India'!S8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!S10/'Revised Calcs_India'!$B$10)</f>
         <v>1769.3289221621408</v>
       </c>
       <c r="X2" s="9">
-        <f>$F$2*('Revised Calcs_India'!T8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!T10/'Revised Calcs_India'!$B$10)</f>
         <v>1808.0100432241513</v>
       </c>
       <c r="Y2" s="9">
-        <f>$F$2*('Revised Calcs_India'!U8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!U10/'Revised Calcs_India'!$B$10)</f>
         <v>1842.7555237634858</v>
       </c>
       <c r="Z2" s="9">
-        <f>$F$2*('Revised Calcs_India'!V8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!V10/'Revised Calcs_India'!$B$10)</f>
         <v>1871.9404612587182</v>
       </c>
       <c r="AA2" s="9">
-        <f>$F$2*('Revised Calcs_India'!W8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!W10/'Revised Calcs_India'!$B$10)</f>
         <v>1887.3875865273442</v>
       </c>
       <c r="AB2" s="9">
-        <f>$F$2*('Revised Calcs_India'!X8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!X10/'Revised Calcs_India'!$B$10)</f>
         <v>1891.0277902279424</v>
       </c>
       <c r="AC2" s="9">
-        <f>$F$2*('Revised Calcs_India'!Y8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!Y10/'Revised Calcs_India'!$B$10)</f>
         <v>1888.4497522448135</v>
       </c>
       <c r="AD2" s="9">
-        <f>$F$2*('Revised Calcs_India'!Z8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!Z10/'Revised Calcs_India'!$B$10)</f>
         <v>1852.0758520790275</v>
       </c>
       <c r="AE2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AA8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AA10/'Revised Calcs_India'!$B$10)</f>
         <v>1813.5178296928827</v>
       </c>
       <c r="AF2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AB8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AB10/'Revised Calcs_India'!$B$10)</f>
         <v>1765.6148592560232</v>
       </c>
       <c r="AG2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AC8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AC10/'Revised Calcs_India'!$B$10)</f>
         <v>1691.6501405858942</v>
       </c>
       <c r="AH2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AD8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AD10/'Revised Calcs_India'!$B$10)</f>
         <v>1627.3433923136811</v>
       </c>
       <c r="AI2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AE8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AE10/'Revised Calcs_India'!$B$10)</f>
         <v>1539.8167166681826</v>
       </c>
       <c r="AJ2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AF8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AF10/'Revised Calcs_India'!$B$10)</f>
         <v>1445.4105835943069</v>
       </c>
       <c r="AK2" s="9">
-        <f>$F$2*('Revised Calcs_India'!AG8/'Revised Calcs_India'!$B$8)</f>
+        <f>$F$2*('Revised Calcs_India'!AG10/'Revised Calcs_India'!$B$10)</f>
         <v>1337.8891658832028</v>
       </c>
     </row>
@@ -3221,8 +3243,8 @@
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3368,127 +3390,127 @@
       </c>
       <c r="G2" s="9">
         <f>FORECAST('DRC-PADRC'!G1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!G2</f>
-        <v>8082.2086517291773</v>
+        <v>6945.8450153640169</v>
       </c>
       <c r="H2" s="9">
         <f>FORECAST('DRC-PADRC'!H1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!H2</f>
-        <v>16116.98914219904</v>
+        <v>13844.261869470582</v>
       </c>
       <c r="I2" s="9">
         <f>FORECAST('DRC-PADRC'!I1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!I2</f>
-        <v>24156.236356052174</v>
+        <v>20747.145446958555</v>
       </c>
       <c r="J2" s="9">
         <f>FORECAST('DRC-PADRC'!J1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!J2</f>
-        <v>32185.301550856846</v>
+        <v>27639.84700539993</v>
       </c>
       <c r="K2" s="9">
         <f>FORECAST('DRC-PADRC'!K1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!K2</f>
-        <v>40232.940577297129</v>
+        <v>34551.122395476916</v>
       </c>
       <c r="L2" s="9">
         <f>FORECAST('DRC-PADRC'!L1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!L2</f>
-        <v>48285.732162598651</v>
+        <v>41467.55034441514</v>
       </c>
       <c r="M2" s="9">
         <f>FORECAST('DRC-PADRC'!M1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!M2</f>
-        <v>56343.44417782977</v>
+        <v>48388.89872328296</v>
       </c>
       <c r="N2" s="9">
         <f>FORECAST('DRC-PADRC'!N1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!N2</f>
-        <v>64404.187937592207</v>
+        <v>55313.2788466821</v>
       </c>
       <c r="O2" s="9">
         <f>FORECAST('DRC-PADRC'!O1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!O2</f>
-        <v>72446.322694668779</v>
+        <v>62219.049967395382</v>
       </c>
       <c r="P2" s="9">
         <f>FORECAST('DRC-PADRC'!P1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!P2</f>
-        <v>80494.155161887291</v>
+        <v>69130.518798248726</v>
       </c>
       <c r="Q2" s="9">
         <f>FORECAST('DRC-PADRC'!Q1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Q2</f>
-        <v>88549.802636468899</v>
+        <v>76049.802636467037</v>
       </c>
       <c r="R2" s="9">
         <f>FORECAST('DRC-PADRC'!R1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!R2</f>
-        <v>96583.169250718813</v>
+        <v>82946.805614353652</v>
       </c>
       <c r="S2" s="9">
         <f>FORECAST('DRC-PADRC'!S1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!S2</f>
-        <v>104624.7799591467</v>
+        <v>89852.052686418247</v>
       </c>
       <c r="T2" s="9">
         <f>FORECAST('DRC-PADRC'!T1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!T2</f>
-        <v>112663.08107174633</v>
+        <v>96753.990162654576</v>
       </c>
       <c r="U2" s="9">
         <f>FORECAST('DRC-PADRC'!U1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!U2</f>
-        <v>120708.65907464211</v>
+        <v>103663.20452918706</v>
       </c>
       <c r="V2" s="9">
         <f>FORECAST('DRC-PADRC'!V1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!V2</f>
-        <v>128759.46349560466</v>
+        <v>110577.64531378631</v>
       </c>
       <c r="W2" s="9">
         <f>FORECAST('DRC-PADRC'!W1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!W2</f>
-        <v>136818.56828442556</v>
+        <v>117500.38646624393</v>
       </c>
       <c r="X2" s="9">
         <f>FORECAST('DRC-PADRC'!X1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!X2</f>
-        <v>144877.87003112974</v>
+        <v>124423.32457658293</v>
       </c>
       <c r="Y2" s="9">
         <f>FORECAST('DRC-PADRC'!Y1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Y2</f>
-        <v>152941.10741835472</v>
+        <v>131350.19832744461</v>
       </c>
       <c r="Z2" s="9">
         <f>FORECAST('DRC-PADRC'!Z1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Z2</f>
-        <v>161009.90534862378</v>
+        <v>138282.63262134852</v>
       </c>
       <c r="AA2" s="9">
         <f>FORECAST('DRC-PADRC'!AA1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AA2</f>
-        <v>169092.44109111946</v>
+        <v>145228.80472748089</v>
       </c>
       <c r="AB2" s="9">
         <f>FORECAST('DRC-PADRC'!AB1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AB2</f>
-        <v>177186.78375518319</v>
+        <v>152186.78375518133</v>
       </c>
       <c r="AC2" s="9">
         <f>FORECAST('DRC-PADRC'!AC1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AC2</f>
-        <v>185287.34466093063</v>
+        <v>159150.98102456547</v>
       </c>
       <c r="AD2" s="9">
         <f>FORECAST('DRC-PADRC'!AD1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AD2</f>
-        <v>193421.70142886072</v>
+        <v>166148.97415613226</v>
       </c>
       <c r="AE2" s="9">
         <f>FORECAST('DRC-PADRC'!AE1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AE2</f>
-        <v>201558.24231901116</v>
+        <v>173149.1514099194</v>
       </c>
       <c r="AF2" s="9">
         <f>FORECAST('DRC-PADRC'!AF1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AF2</f>
-        <v>209704.1281572142</v>
+        <v>180158.67361175729</v>
       </c>
       <c r="AG2" s="9">
         <f>FORECAST('DRC-PADRC'!AG1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AG2</f>
-        <v>217876.07574364863</v>
+        <v>187194.25756182842</v>
       </c>
       <c r="AH2" s="9">
         <f>FORECAST('DRC-PADRC'!AH1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AH2</f>
-        <v>226038.36535968515</v>
+        <v>194220.18354150164</v>
       </c>
       <c r="AI2" s="9">
         <f>FORECAST('DRC-PADRC'!AI1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AI2</f>
-        <v>234223.87490309495</v>
+        <v>201269.32944854815</v>
       </c>
       <c r="AJ2" s="9">
         <f>FORECAST('DRC-PADRC'!AJ1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AJ2</f>
-        <v>242416.26390393314</v>
+        <v>208325.35481302303</v>
       </c>
       <c r="AK2" s="9">
         <f>FORECAST('DRC-PADRC'!AK1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AK2</f>
-        <v>250621.76818940855</v>
+        <v>215394.49546213515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DRC based on peak power demand
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -262,12 +262,6 @@
     <t>Time (Year)</t>
   </si>
   <si>
-    <t>Peak Power Demand after Storage and DR[summer] : MostRecentRun</t>
-  </si>
-  <si>
-    <t>Peak Power Demand after Storage and DR[winter] : MostRecentRun</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t>is calculated separately in the EPS.</t>
+  </si>
+  <si>
+    <t>Peak Hour Electricity Demand by Season[summer] : NoSettings</t>
+  </si>
+  <si>
+    <t>Peak Hour Electricity Demand by Season[winter] : NoSettings</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1288,10 +1288,10 @@
         <v>53</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -1299,7 +1299,7 @@
         <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -1315,7 +1315,7 @@
         <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -1323,7 +1323,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -1331,12 +1331,12 @@
         <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -1423,19 +1423,19 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B32" s="6"/>
     </row>
@@ -1445,13 +1445,13 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="6"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="6"/>
     </row>
@@ -1506,7 +1506,7 @@
   <dimension ref="A1:AG29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1518,22 +1518,22 @@
   <sheetData>
     <row r="1" spans="1:33" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B1" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>81</v>
-      </c>
       <c r="K1" s="52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
@@ -1547,7 +1547,7 @@
         <v>2030</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I2" s="53">
         <v>40</v>
@@ -1575,22 +1575,22 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="G4" s="51" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.45">
       <c r="G5" s="51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.45">
       <c r="G6" s="51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.45">
       <c r="G7" s="51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.45">
@@ -1699,209 +1699,209 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B10">
-        <v>262201</v>
+        <v>164581</v>
       </c>
       <c r="C10">
-        <v>266686</v>
+        <v>167124</v>
       </c>
       <c r="D10">
-        <v>284656</v>
+        <v>184567</v>
       </c>
       <c r="E10">
-        <v>301356</v>
+        <v>199680</v>
       </c>
       <c r="F10">
-        <v>320951</v>
+        <v>216498</v>
       </c>
       <c r="G10">
-        <v>335265</v>
+        <v>232792</v>
       </c>
       <c r="H10">
-        <v>348114</v>
+        <v>248850</v>
       </c>
       <c r="I10">
-        <v>359564</v>
+        <v>264673</v>
       </c>
       <c r="J10">
-        <v>370152</v>
+        <v>280541</v>
       </c>
       <c r="K10">
-        <v>386031</v>
+        <v>302367</v>
       </c>
       <c r="L10">
-        <v>400290</v>
+        <v>324258</v>
       </c>
       <c r="M10">
-        <v>412327</v>
+        <v>346278</v>
       </c>
       <c r="N10">
-        <v>430699</v>
+        <v>368229</v>
       </c>
       <c r="O10">
-        <v>446727</v>
+        <v>390186</v>
       </c>
       <c r="P10">
-        <v>463696</v>
+        <v>414236</v>
       </c>
       <c r="Q10">
-        <v>478596</v>
+        <v>438370</v>
       </c>
       <c r="R10">
-        <v>492010</v>
+        <v>462533</v>
       </c>
       <c r="S10">
-        <v>503064</v>
+        <v>486619</v>
       </c>
       <c r="T10">
-        <v>514062</v>
+        <v>511017</v>
       </c>
       <c r="U10">
-        <v>523941</v>
+        <v>535347</v>
       </c>
       <c r="V10">
-        <v>532239</v>
+        <v>559541</v>
       </c>
       <c r="W10">
-        <v>536631</v>
+        <v>584045</v>
       </c>
       <c r="X10">
-        <v>537666</v>
+        <v>608681</v>
       </c>
       <c r="Y10">
-        <v>536933</v>
+        <v>633204</v>
       </c>
       <c r="Z10">
-        <v>526591</v>
+        <v>653169</v>
       </c>
       <c r="AA10">
-        <v>515628</v>
+        <v>675065</v>
       </c>
       <c r="AB10">
-        <v>502008</v>
+        <v>695867</v>
       </c>
       <c r="AC10">
-        <v>480978</v>
+        <v>715551</v>
       </c>
       <c r="AD10">
-        <v>462694</v>
+        <v>737951</v>
       </c>
       <c r="AE10">
-        <v>437808</v>
+        <v>757599</v>
       </c>
       <c r="AF10">
-        <v>410966</v>
+        <v>778490</v>
       </c>
       <c r="AG10">
-        <v>380395</v>
+        <v>799341</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B11">
-        <v>173800</v>
+        <v>144301</v>
       </c>
       <c r="C11">
-        <v>171183</v>
+        <v>144210</v>
       </c>
       <c r="D11">
-        <v>179976</v>
+        <v>157047</v>
       </c>
       <c r="E11">
-        <v>190340</v>
+        <v>167875</v>
       </c>
       <c r="F11">
-        <v>200057</v>
+        <v>178025</v>
       </c>
       <c r="G11">
-        <v>207445</v>
+        <v>187719</v>
       </c>
       <c r="H11">
-        <v>214344</v>
+        <v>197150</v>
       </c>
       <c r="I11">
-        <v>220464</v>
+        <v>206417</v>
       </c>
       <c r="J11">
-        <v>226506</v>
+        <v>215696</v>
       </c>
       <c r="K11">
-        <v>230307</v>
+        <v>226630</v>
       </c>
       <c r="L11">
-        <v>233659</v>
+        <v>237552</v>
       </c>
       <c r="M11">
-        <v>235732</v>
+        <v>248582</v>
       </c>
       <c r="N11">
-        <v>244440</v>
+        <v>259703</v>
       </c>
       <c r="O11">
-        <v>253558</v>
+        <v>270844</v>
       </c>
       <c r="P11">
-        <v>261443</v>
+        <v>283077</v>
       </c>
       <c r="Q11">
-        <v>268575</v>
+        <v>295421</v>
       </c>
       <c r="R11">
-        <v>275152</v>
+        <v>307771</v>
       </c>
       <c r="S11">
-        <v>281129</v>
+        <v>320177</v>
       </c>
       <c r="T11">
-        <v>286490</v>
+        <v>332695</v>
       </c>
       <c r="U11">
-        <v>292265</v>
+        <v>346994</v>
       </c>
       <c r="V11">
-        <v>297605</v>
+        <v>361314</v>
       </c>
       <c r="W11">
-        <v>300694</v>
+        <v>375578</v>
       </c>
       <c r="X11">
-        <v>301757</v>
+        <v>390049</v>
       </c>
       <c r="Y11">
-        <v>302059</v>
+        <v>404517</v>
       </c>
       <c r="Z11">
-        <v>297336</v>
+        <v>416752</v>
       </c>
       <c r="AA11">
-        <v>290606</v>
+        <v>428795</v>
       </c>
       <c r="AB11">
-        <v>283666</v>
+        <v>441039</v>
       </c>
       <c r="AC11">
-        <v>273523</v>
+        <v>453324</v>
       </c>
       <c r="AD11">
-        <v>263033</v>
+        <v>465684</v>
       </c>
       <c r="AE11">
-        <v>250773</v>
+        <v>477938</v>
       </c>
       <c r="AF11">
-        <v>236428</v>
+        <v>490292</v>
       </c>
       <c r="AG11">
-        <v>220010</v>
+        <v>502594</v>
       </c>
     </row>
     <row r="29" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G29" s="51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3103,127 +3103,127 @@
       </c>
       <c r="G2" s="9">
         <f>$F$2*('Revised Calcs_India'!C10/'Revised Calcs_India'!$B$10)</f>
-        <v>937.96267062587003</v>
+        <v>936.4375188198502</v>
       </c>
       <c r="H2" s="9">
         <f>$F$2*('Revised Calcs_India'!D10/'Revised Calcs_India'!$B$10)</f>
-        <v>1001.1650479203171</v>
+        <v>1034.1750050024132</v>
       </c>
       <c r="I2" s="9">
         <f>$F$2*('Revised Calcs_India'!E10/'Revised Calcs_India'!$B$10)</f>
-        <v>1059.9007018333534</v>
+        <v>1118.856919161507</v>
       </c>
       <c r="J2" s="9">
         <f>$F$2*('Revised Calcs_India'!F10/'Revised Calcs_India'!$B$10)</f>
-        <v>1128.8183747929911</v>
+        <v>1213.0923742218947</v>
       </c>
       <c r="K2" s="9">
         <f>$F$2*('Revised Calcs_India'!G10/'Revised Calcs_India'!$B$10)</f>
-        <v>1179.1622161170153</v>
+        <v>1304.3917263894509</v>
       </c>
       <c r="L2" s="9">
         <f>$F$2*('Revised Calcs_India'!H10/'Revised Calcs_India'!$B$10)</f>
-        <v>1224.353498579806</v>
+        <v>1394.3687116052736</v>
       </c>
       <c r="M2" s="9">
         <f>$F$2*('Revised Calcs_India'!I10/'Revised Calcs_India'!$B$10)</f>
-        <v>1264.6243511129956</v>
+        <v>1483.0289331191582</v>
       </c>
       <c r="N2" s="9">
         <f>$F$2*('Revised Calcs_India'!J10/'Revised Calcs_India'!$B$10)</f>
-        <v>1301.8634591148657</v>
+        <v>1571.94130087384</v>
       </c>
       <c r="O2" s="9">
         <f>$F$2*('Revised Calcs_India'!K10/'Revised Calcs_India'!$B$10)</f>
-        <v>1357.7115698025964</v>
+        <v>1694.2378309099929</v>
       </c>
       <c r="P2" s="9">
         <f>$F$2*('Revised Calcs_India'!L10/'Revised Calcs_India'!$B$10)</f>
-        <v>1407.8619703502604</v>
+        <v>1816.8985721828521</v>
       </c>
       <c r="Q2" s="9">
         <f>$F$2*('Revised Calcs_India'!M10/'Revised Calcs_India'!$B$10)</f>
-        <v>1450.1973635329682</v>
+        <v>1940.2821326793287</v>
       </c>
       <c r="R2" s="9">
         <f>$F$2*('Revised Calcs_India'!N10/'Revised Calcs_India'!$B$10)</f>
-        <v>1514.8136170473576</v>
+        <v>2063.2790689399167</v>
       </c>
       <c r="S2" s="9">
         <f>$F$2*('Revised Calcs_India'!O10/'Revised Calcs_India'!$B$10)</f>
-        <v>1571.1857763837736</v>
+        <v>2186.3096246992777</v>
       </c>
       <c r="T2" s="9">
         <f>$F$2*('Revised Calcs_India'!P10/'Revised Calcs_India'!$B$10)</f>
-        <v>1630.8675315484631</v>
+        <v>2321.0677822805787</v>
       </c>
       <c r="U2" s="9">
         <f>$F$2*('Revised Calcs_India'!Q10/'Revised Calcs_India'!$B$10)</f>
-        <v>1683.2723964169807</v>
+        <v>2456.2966128447006</v>
       </c>
       <c r="V2" s="9">
         <f>$F$2*('Revised Calcs_India'!R10/'Revised Calcs_India'!$B$10)</f>
-        <v>1730.4508432187454</v>
+        <v>2591.6879376528914</v>
       </c>
       <c r="W2" s="9">
         <f>$F$2*('Revised Calcs_India'!S10/'Revised Calcs_India'!$B$10)</f>
-        <v>1769.3289221621408</v>
+        <v>2726.64781222683</v>
       </c>
       <c r="X2" s="9">
         <f>$F$2*('Revised Calcs_India'!T10/'Revised Calcs_India'!$B$10)</f>
-        <v>1808.0100432241513</v>
+        <v>2863.3559007369581</v>
       </c>
       <c r="Y2" s="9">
         <f>$F$2*('Revised Calcs_India'!U10/'Revised Calcs_India'!$B$10)</f>
-        <v>1842.7555237634858</v>
+        <v>2999.6829682609937</v>
       </c>
       <c r="Z2" s="9">
         <f>$F$2*('Revised Calcs_India'!V10/'Revised Calcs_India'!$B$10)</f>
-        <v>1871.9404612587182</v>
+        <v>3135.2479938128445</v>
       </c>
       <c r="AA2" s="9">
         <f>$F$2*('Revised Calcs_India'!W10/'Revised Calcs_India'!$B$10)</f>
-        <v>1887.3875865273442</v>
+        <v>3272.5500268012938</v>
       </c>
       <c r="AB2" s="9">
         <f>$F$2*('Revised Calcs_India'!X10/'Revised Calcs_India'!$B$10)</f>
-        <v>1891.0277902279424</v>
+        <v>3410.5916887627463</v>
       </c>
       <c r="AC2" s="9">
         <f>$F$2*('Revised Calcs_India'!Y10/'Revised Calcs_India'!$B$10)</f>
-        <v>1888.4497522448135</v>
+        <v>3548.00018349731</v>
       </c>
       <c r="AD2" s="9">
         <f>$F$2*('Revised Calcs_India'!Z10/'Revised Calcs_India'!$B$10)</f>
-        <v>1852.0758520790275</v>
+        <v>3659.8690656640747</v>
       </c>
       <c r="AE2" s="9">
         <f>$F$2*('Revised Calcs_India'!AA10/'Revised Calcs_India'!$B$10)</f>
-        <v>1813.5178296928827</v>
+        <v>3782.5578231859113</v>
       </c>
       <c r="AF2" s="9">
         <f>$F$2*('Revised Calcs_India'!AB10/'Revised Calcs_India'!$B$10)</f>
-        <v>1765.6148592560232</v>
+        <v>3899.1166254314926</v>
       </c>
       <c r="AG2" s="9">
         <f>$F$2*('Revised Calcs_India'!AC10/'Revised Calcs_India'!$B$10)</f>
-        <v>1691.6501405858942</v>
+        <v>4009.4109944057273</v>
       </c>
       <c r="AH2" s="9">
         <f>$F$2*('Revised Calcs_India'!AD10/'Revised Calcs_India'!$B$10)</f>
-        <v>1627.3433923136811</v>
+        <v>4134.9237898244855</v>
       </c>
       <c r="AI2" s="9">
         <f>$F$2*('Revised Calcs_India'!AE10/'Revised Calcs_India'!$B$10)</f>
-        <v>1539.8167166681826</v>
+        <v>4245.0164418060831</v>
       </c>
       <c r="AJ2" s="9">
         <f>$F$2*('Revised Calcs_India'!AF10/'Revised Calcs_India'!$B$10)</f>
-        <v>1445.4105835943069</v>
+        <v>4362.0739332834619</v>
       </c>
       <c r="AK2" s="9">
         <f>$F$2*('Revised Calcs_India'!AG10/'Revised Calcs_India'!$B$10)</f>
-        <v>1337.8891658832028</v>
+        <v>4478.9072947690211</v>
       </c>
     </row>
   </sheetData>
@@ -3390,127 +3390,127 @@
       </c>
       <c r="G2" s="9">
         <f>FORECAST('DRC-PADRC'!G1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!G2</f>
-        <v>6945.8450153640169</v>
+        <v>6947.3701671700364</v>
       </c>
       <c r="H2" s="9">
         <f>FORECAST('DRC-PADRC'!H1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!H2</f>
-        <v>13844.261869470582</v>
+        <v>13811.251912388485</v>
       </c>
       <c r="I2" s="9">
         <f>FORECAST('DRC-PADRC'!I1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!I2</f>
-        <v>20747.145446958555</v>
+        <v>20688.189229630403</v>
       </c>
       <c r="J2" s="9">
         <f>FORECAST('DRC-PADRC'!J1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!J2</f>
-        <v>27639.84700539993</v>
+        <v>27555.573005971026</v>
       </c>
       <c r="K2" s="9">
         <f>FORECAST('DRC-PADRC'!K1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!K2</f>
-        <v>34551.122395476916</v>
+        <v>34425.892885204477</v>
       </c>
       <c r="L2" s="9">
         <f>FORECAST('DRC-PADRC'!L1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!L2</f>
-        <v>41467.55034441514</v>
+        <v>41297.535131389668</v>
       </c>
       <c r="M2" s="9">
         <f>FORECAST('DRC-PADRC'!M1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!M2</f>
-        <v>48388.89872328296</v>
+        <v>48170.494141276795</v>
       </c>
       <c r="N2" s="9">
         <f>FORECAST('DRC-PADRC'!N1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!N2</f>
-        <v>55313.2788466821</v>
+        <v>55043.201004923125</v>
       </c>
       <c r="O2" s="9">
         <f>FORECAST('DRC-PADRC'!O1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!O2</f>
-        <v>62219.049967395382</v>
+        <v>61882.523706287982</v>
       </c>
       <c r="P2" s="9">
         <f>FORECAST('DRC-PADRC'!P1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!P2</f>
-        <v>69130.518798248726</v>
+        <v>68721.482196416138</v>
       </c>
       <c r="Q2" s="9">
         <f>FORECAST('DRC-PADRC'!Q1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Q2</f>
-        <v>76049.802636467037</v>
+        <v>75559.717867320665</v>
       </c>
       <c r="R2" s="9">
         <f>FORECAST('DRC-PADRC'!R1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!R2</f>
-        <v>82946.805614353652</v>
+        <v>82398.3401624611</v>
       </c>
       <c r="S2" s="9">
         <f>FORECAST('DRC-PADRC'!S1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!S2</f>
-        <v>89852.052686418247</v>
+        <v>89236.928838102744</v>
       </c>
       <c r="T2" s="9">
         <f>FORECAST('DRC-PADRC'!T1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!T2</f>
-        <v>96753.990162654576</v>
+        <v>96063.78991192246</v>
       </c>
       <c r="U2" s="9">
         <f>FORECAST('DRC-PADRC'!U1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!U2</f>
-        <v>103663.20452918706</v>
+        <v>102890.18031275934</v>
       </c>
       <c r="V2" s="9">
         <f>FORECAST('DRC-PADRC'!V1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!V2</f>
-        <v>110577.64531378631</v>
+        <v>109716.40821935216</v>
       </c>
       <c r="W2" s="9">
         <f>FORECAST('DRC-PADRC'!W1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!W2</f>
-        <v>117500.38646624393</v>
+        <v>116543.06757617924</v>
       </c>
       <c r="X2" s="9">
         <f>FORECAST('DRC-PADRC'!X1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!X2</f>
-        <v>124423.32457658293</v>
+        <v>123367.97871907012</v>
       </c>
       <c r="Y2" s="9">
         <f>FORECAST('DRC-PADRC'!Y1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Y2</f>
-        <v>131350.19832744461</v>
+        <v>130193.27088294709</v>
       </c>
       <c r="Z2" s="9">
         <f>FORECAST('DRC-PADRC'!Z1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Z2</f>
-        <v>138282.63262134852</v>
+        <v>137019.3250887944</v>
       </c>
       <c r="AA2" s="9">
         <f>FORECAST('DRC-PADRC'!AA1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AA2</f>
-        <v>145228.80472748089</v>
+        <v>143843.64228720695</v>
       </c>
       <c r="AB2" s="9">
         <f>FORECAST('DRC-PADRC'!AB1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AB2</f>
-        <v>152186.78375518133</v>
+        <v>150667.21985664652</v>
       </c>
       <c r="AC2" s="9">
         <f>FORECAST('DRC-PADRC'!AC1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AC2</f>
-        <v>159150.98102456547</v>
+        <v>157491.43059331295</v>
       </c>
       <c r="AD2" s="9">
         <f>FORECAST('DRC-PADRC'!AD1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AD2</f>
-        <v>166148.97415613226</v>
+        <v>164341.18094254722</v>
       </c>
       <c r="AE2" s="9">
         <f>FORECAST('DRC-PADRC'!AE1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AE2</f>
-        <v>173149.1514099194</v>
+        <v>171180.11141642637</v>
       </c>
       <c r="AF2" s="9">
         <f>FORECAST('DRC-PADRC'!AF1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AF2</f>
-        <v>180158.67361175729</v>
+        <v>178025.17184558182</v>
       </c>
       <c r="AG2" s="9">
         <f>FORECAST('DRC-PADRC'!AG1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AG2</f>
-        <v>187194.25756182842</v>
+        <v>184876.49670800858</v>
       </c>
       <c r="AH2" s="9">
         <f>FORECAST('DRC-PADRC'!AH1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AH2</f>
-        <v>194220.18354150164</v>
+        <v>191712.60314399085</v>
       </c>
       <c r="AI2" s="9">
         <f>FORECAST('DRC-PADRC'!AI1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AI2</f>
-        <v>201269.32944854815</v>
+        <v>198564.12972341027</v>
       </c>
       <c r="AJ2" s="9">
         <f>FORECAST('DRC-PADRC'!AJ1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AJ2</f>
-        <v>208325.35481302303</v>
+        <v>205408.6914633339</v>
       </c>
       <c r="AK2" s="9">
         <f>FORECAST('DRC-PADRC'!AK1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AK2</f>
-        <v>215394.49546213515</v>
+        <v>212253.47733324935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recalculate DRC based on peak demand
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\elec\DRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5B4319-C43C-423C-A856-9F290C37B2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="4590"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="DRC-BDRC" sheetId="5" r:id="rId4"/>
     <sheet name="DRC-PADRC" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -259,9 +262,6 @@
     <t>periods in response to time-based rates or other financial incentives.</t>
   </si>
   <si>
-    <t>Time (Year)</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -336,16 +336,19 @@
     <t>is calculated separately in the EPS.</t>
   </si>
   <si>
-    <t>Peak Hour Electricity Demand by Season[summer] : NoSettings</t>
-  </si>
-  <si>
-    <t>Peak Hour Electricity Demand by Season[winter] : NoSettings</t>
+    <t>Time (Time)</t>
+  </si>
+  <si>
+    <t>Peak Hour Electricity Demand by Season[summer] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>Peak Hour Electricity Demand by Season[winter] : MostRecentRun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1050,6 +1053,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1085,6 +1105,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1260,49 +1297,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="7" max="7" width="51.265625" customWidth="1"/>
+    <col min="7" max="7" width="51.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>2015</v>
       </c>
@@ -1310,186 +1347,186 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" s="33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="5"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="B22" r:id="rId2"/>
-    <hyperlink ref="G8" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
@@ -1502,41 +1539,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" customWidth="1"/>
-    <col min="8" max="8" width="18.86328125" customWidth="1"/>
+    <col min="1" max="1" width="63.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B1" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="52" t="s">
+      <c r="K1" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1584,7 @@
         <v>2030</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="53">
         <v>40</v>
@@ -1560,7 +1597,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1573,32 +1610,32 @@
         <v>77500</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="G4" s="51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="G5" s="51" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="G5" s="51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="G6" s="51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="G7" s="51" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="G7" s="51" t="s">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="G8" s="51"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="G8" s="51"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>66</v>
       </c>
       <c r="B9">
         <v>2019</v>
@@ -1697,211 +1734,211 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>91</v>
       </c>
       <c r="B10">
-        <v>164581</v>
+        <v>162417</v>
       </c>
       <c r="C10">
-        <v>167124</v>
+        <v>161230</v>
       </c>
       <c r="D10">
-        <v>184567</v>
+        <v>174773</v>
       </c>
       <c r="E10">
-        <v>199680</v>
+        <v>185487</v>
       </c>
       <c r="F10">
-        <v>216498</v>
+        <v>195731</v>
       </c>
       <c r="G10">
-        <v>232792</v>
+        <v>205399</v>
       </c>
       <c r="H10">
-        <v>248850</v>
+        <v>214078</v>
       </c>
       <c r="I10">
-        <v>264673</v>
+        <v>222460</v>
       </c>
       <c r="J10">
-        <v>280541</v>
+        <v>231463</v>
       </c>
       <c r="K10">
-        <v>302367</v>
+        <v>243188</v>
       </c>
       <c r="L10">
-        <v>324258</v>
+        <v>255060</v>
       </c>
       <c r="M10">
-        <v>346278</v>
+        <v>266853</v>
       </c>
       <c r="N10">
-        <v>368229</v>
+        <v>282041</v>
       </c>
       <c r="O10">
-        <v>390186</v>
+        <v>297497</v>
       </c>
       <c r="P10">
-        <v>414236</v>
+        <v>313255</v>
       </c>
       <c r="Q10">
-        <v>438370</v>
+        <v>328972</v>
       </c>
       <c r="R10">
-        <v>462533</v>
+        <v>344356</v>
       </c>
       <c r="S10">
-        <v>486619</v>
+        <v>359267</v>
       </c>
       <c r="T10">
-        <v>511017</v>
+        <v>373991</v>
       </c>
       <c r="U10">
-        <v>535347</v>
+        <v>389229</v>
       </c>
       <c r="V10">
-        <v>559541</v>
+        <v>404542</v>
       </c>
       <c r="W10">
-        <v>584045</v>
+        <v>419785</v>
       </c>
       <c r="X10">
-        <v>608681</v>
+        <v>434919</v>
       </c>
       <c r="Y10">
-        <v>633204</v>
+        <v>449155</v>
       </c>
       <c r="Z10">
-        <v>653169</v>
+        <v>461626</v>
       </c>
       <c r="AA10">
-        <v>675065</v>
+        <v>473803</v>
       </c>
       <c r="AB10">
-        <v>695867</v>
+        <v>485708</v>
       </c>
       <c r="AC10">
-        <v>715551</v>
+        <v>497094</v>
       </c>
       <c r="AD10">
-        <v>737951</v>
+        <v>508145</v>
       </c>
       <c r="AE10">
-        <v>757599</v>
+        <v>518988</v>
       </c>
       <c r="AF10">
-        <v>778490</v>
+        <v>529610</v>
       </c>
       <c r="AG10">
-        <v>799341</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.45">
+        <v>539807</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>92</v>
       </c>
       <c r="B11">
-        <v>144301</v>
+        <v>146544</v>
       </c>
       <c r="C11">
-        <v>144210</v>
+        <v>144093</v>
       </c>
       <c r="D11">
-        <v>157047</v>
+        <v>154638</v>
       </c>
       <c r="E11">
-        <v>167875</v>
+        <v>162791</v>
       </c>
       <c r="F11">
-        <v>178025</v>
+        <v>169782</v>
       </c>
       <c r="G11">
-        <v>187719</v>
+        <v>176290</v>
       </c>
       <c r="H11">
-        <v>197150</v>
+        <v>182072</v>
       </c>
       <c r="I11">
-        <v>206417</v>
+        <v>187784</v>
       </c>
       <c r="J11">
-        <v>215696</v>
+        <v>193901</v>
       </c>
       <c r="K11">
-        <v>226630</v>
+        <v>200803</v>
       </c>
       <c r="L11">
-        <v>237552</v>
+        <v>207926</v>
       </c>
       <c r="M11">
-        <v>248582</v>
+        <v>214997</v>
       </c>
       <c r="N11">
-        <v>259703</v>
+        <v>225052</v>
       </c>
       <c r="O11">
-        <v>270844</v>
+        <v>235281</v>
       </c>
       <c r="P11">
-        <v>283077</v>
+        <v>246160</v>
       </c>
       <c r="Q11">
-        <v>295421</v>
+        <v>256970</v>
       </c>
       <c r="R11">
-        <v>307771</v>
+        <v>267780</v>
       </c>
       <c r="S11">
-        <v>320177</v>
+        <v>278181</v>
       </c>
       <c r="T11">
-        <v>332695</v>
+        <v>288508</v>
       </c>
       <c r="U11">
-        <v>346994</v>
+        <v>299929</v>
       </c>
       <c r="V11">
-        <v>361314</v>
+        <v>311352</v>
       </c>
       <c r="W11">
-        <v>375578</v>
+        <v>322904</v>
       </c>
       <c r="X11">
-        <v>390049</v>
+        <v>334325</v>
       </c>
       <c r="Y11">
-        <v>404517</v>
+        <v>345221</v>
       </c>
       <c r="Z11">
-        <v>416752</v>
+        <v>354663</v>
       </c>
       <c r="AA11">
-        <v>428795</v>
+        <v>363924</v>
       </c>
       <c r="AB11">
-        <v>441039</v>
+        <v>373016</v>
       </c>
       <c r="AC11">
-        <v>453324</v>
+        <v>381915</v>
       </c>
       <c r="AD11">
-        <v>465684</v>
+        <v>390538</v>
       </c>
       <c r="AE11">
-        <v>477938</v>
+        <v>399059</v>
       </c>
       <c r="AF11">
-        <v>490292</v>
+        <v>407410</v>
       </c>
       <c r="AG11">
-        <v>502594</v>
-      </c>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.45">
+        <v>415558</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G29" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1912,31 +1949,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK99"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68.73046875" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.265625" customWidth="1"/>
+    <col min="1" max="1" width="68.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1956,7 +1993,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1976,7 +2013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1996,7 +2033,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2052,7 +2089,7 @@
       <c r="AJ6" s="12"/>
       <c r="AK6" s="12"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2104,7 +2141,7 @@
       <c r="AJ7" s="13"/>
       <c r="AK7" s="13"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2160,7 +2197,7 @@
       <c r="AJ8" s="9"/>
       <c r="AK8" s="9"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2168,7 +2205,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2176,7 +2213,7 @@
         <v>5.77</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -2214,7 +2251,7 @@
       <c r="AJ12" s="9"/>
       <c r="AK12" s="9"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2260,7 +2297,7 @@
       <c r="AJ13" s="9"/>
       <c r="AK13" s="9"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -2295,7 +2332,7 @@
       <c r="AJ14" s="9"/>
       <c r="AK14" s="9"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2337,7 +2374,7 @@
       <c r="AJ15" s="9"/>
       <c r="AK15" s="9"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -2372,7 +2409,7 @@
       <c r="AJ16" s="9"/>
       <c r="AK16" s="9"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2381,27 +2418,27 @@
         <v>6.5902592944698366</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K65" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B75" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -2416,7 +2453,7 @@
       <c r="K78" s="54"/>
       <c r="L78" s="54"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="55" t="s">
         <v>0</v>
       </c>
@@ -2445,7 +2482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="56"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -2462,7 +2499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="57"/>
       <c r="B81" s="20"/>
       <c r="C81" s="20"/>
@@ -2479,7 +2516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="23">
         <v>1</v>
       </c>
@@ -2508,7 +2545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="36" t="s">
         <v>27</v>
       </c>
@@ -2537,7 +2574,7 @@
         <v>553995</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="36" t="s">
         <v>28</v>
       </c>
@@ -2566,7 +2603,7 @@
         <v>612644.98941921792</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="36" t="s">
         <v>29</v>
       </c>
@@ -2595,7 +2632,7 @@
         <v>694392</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="39" t="s">
         <v>30</v>
       </c>
@@ -2624,7 +2661,7 @@
         <v>785194</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="39" t="s">
         <v>31</v>
       </c>
@@ -2653,7 +2690,7 @@
         <v>824300.99</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="40" t="s">
         <v>32</v>
       </c>
@@ -2682,7 +2719,7 @@
         <v>874208.56649999996</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="40" t="s">
         <v>33</v>
       </c>
@@ -2711,7 +2748,7 @@
         <v>948521.67230967898</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="40" t="s">
         <v>34</v>
       </c>
@@ -2740,7 +2777,7 @@
         <v>1001190.6843085778</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="40" t="s">
         <v>58</v>
       </c>
@@ -2769,7 +2806,7 @@
         <v>1061182.6382699322</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="41" t="s">
         <v>59</v>
       </c>
@@ -2798,7 +2835,7 @@
         <v>1130243.8375010479</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="27" t="s">
         <v>35</v>
       </c>
@@ -2827,7 +2864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="45" t="s">
         <v>60</v>
       </c>
@@ -2856,7 +2893,7 @@
         <v>6.5079465815335542</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="47" t="s">
         <v>61</v>
       </c>
@@ -2885,7 +2922,7 @@
         <v>7.3906893769725812</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="30" t="s">
         <v>36</v>
       </c>
@@ -2900,7 +2937,7 @@
       <c r="J96" s="31"/>
       <c r="K96" s="31"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="30" t="s">
         <v>37</v>
       </c>
@@ -2915,7 +2952,7 @@
       <c r="J97" s="30"/>
       <c r="K97" s="30"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>63</v>
       </c>
@@ -2931,9 +2968,9 @@
     <mergeCell ref="J79:J81"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A40" r:id="rId1"/>
-    <hyperlink ref="B75" r:id="rId2"/>
-    <hyperlink ref="K65" r:id="rId3"/>
+    <hyperlink ref="A40" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B75" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="K65" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2947,7 +2984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -2957,14 +2994,14 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="37" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="37" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3077,7 +3114,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3103,127 +3140,127 @@
       </c>
       <c r="G2" s="9">
         <f>$F$2*('Revised Calcs_India'!C10/'Revised Calcs_India'!$B$10)</f>
-        <v>936.4375188198502</v>
+        <v>915.44878019872704</v>
       </c>
       <c r="H2" s="9">
         <f>$F$2*('Revised Calcs_India'!D10/'Revised Calcs_India'!$B$10)</f>
-        <v>1034.1750050024132</v>
+        <v>992.34466080550828</v>
       </c>
       <c r="I2" s="9">
         <f>$F$2*('Revised Calcs_India'!E10/'Revised Calcs_India'!$B$10)</f>
-        <v>1118.856919161507</v>
+        <v>1053.1777454116559</v>
       </c>
       <c r="J2" s="9">
         <f>$F$2*('Revised Calcs_India'!F10/'Revised Calcs_India'!$B$10)</f>
-        <v>1213.0923742218947</v>
+        <v>1111.3422142099921</v>
       </c>
       <c r="K2" s="9">
         <f>$F$2*('Revised Calcs_India'!G10/'Revised Calcs_India'!$B$10)</f>
-        <v>1304.3917263894509</v>
+        <v>1166.2362091672662</v>
       </c>
       <c r="L2" s="9">
         <f>$F$2*('Revised Calcs_India'!H10/'Revised Calcs_India'!$B$10)</f>
-        <v>1394.3687116052736</v>
+        <v>1215.5147551161886</v>
       </c>
       <c r="M2" s="9">
         <f>$F$2*('Revised Calcs_India'!I10/'Revised Calcs_India'!$B$10)</f>
-        <v>1483.0289331191582</v>
+        <v>1263.1069629908131</v>
       </c>
       <c r="N2" s="9">
         <f>$F$2*('Revised Calcs_India'!J10/'Revised Calcs_India'!$B$10)</f>
-        <v>1571.94130087384</v>
+        <v>1314.2251504753331</v>
       </c>
       <c r="O2" s="9">
         <f>$F$2*('Revised Calcs_India'!K10/'Revised Calcs_India'!$B$10)</f>
-        <v>1694.2378309099929</v>
+        <v>1380.7985980212616</v>
       </c>
       <c r="P2" s="9">
         <f>$F$2*('Revised Calcs_India'!L10/'Revised Calcs_India'!$B$10)</f>
-        <v>1816.8985721828521</v>
+        <v>1448.2066977453781</v>
       </c>
       <c r="Q2" s="9">
         <f>$F$2*('Revised Calcs_India'!M10/'Revised Calcs_India'!$B$10)</f>
-        <v>1940.2821326793287</v>
+        <v>1515.1662428975433</v>
       </c>
       <c r="R2" s="9">
         <f>$F$2*('Revised Calcs_India'!N10/'Revised Calcs_India'!$B$10)</f>
-        <v>2063.2790689399167</v>
+        <v>1601.4022788316638</v>
       </c>
       <c r="S2" s="9">
         <f>$F$2*('Revised Calcs_India'!O10/'Revised Calcs_India'!$B$10)</f>
-        <v>2186.3096246992777</v>
+        <v>1689.1599935668341</v>
       </c>
       <c r="T2" s="9">
         <f>$F$2*('Revised Calcs_India'!P10/'Revised Calcs_India'!$B$10)</f>
-        <v>2321.0677822805787</v>
+        <v>1778.6324359061725</v>
       </c>
       <c r="U2" s="9">
         <f>$F$2*('Revised Calcs_India'!Q10/'Revised Calcs_India'!$B$10)</f>
-        <v>2456.2966128447006</v>
+        <v>1867.8720841005743</v>
       </c>
       <c r="V2" s="9">
         <f>$F$2*('Revised Calcs_India'!R10/'Revised Calcs_India'!$B$10)</f>
-        <v>2591.6879376528914</v>
+        <v>1955.220989605612</v>
       </c>
       <c r="W2" s="9">
         <f>$F$2*('Revised Calcs_India'!S10/'Revised Calcs_India'!$B$10)</f>
-        <v>2726.64781222683</v>
+        <v>2039.8842455849162</v>
       </c>
       <c r="X2" s="9">
         <f>$F$2*('Revised Calcs_India'!T10/'Revised Calcs_India'!$B$10)</f>
-        <v>2863.3559007369581</v>
+        <v>2123.4857331470703</v>
       </c>
       <c r="Y2" s="9">
         <f>$F$2*('Revised Calcs_India'!U10/'Revised Calcs_India'!$B$10)</f>
-        <v>2999.6829682609937</v>
+        <v>2210.0056643798939</v>
       </c>
       <c r="Z2" s="9">
         <f>$F$2*('Revised Calcs_India'!V10/'Revised Calcs_India'!$B$10)</f>
-        <v>3135.2479938128445</v>
+        <v>2296.9514385607727</v>
       </c>
       <c r="AA2" s="9">
         <f>$F$2*('Revised Calcs_India'!W10/'Revised Calcs_India'!$B$10)</f>
-        <v>3272.5500268012938</v>
+        <v>2383.4997593234671</v>
       </c>
       <c r="AB2" s="9">
         <f>$F$2*('Revised Calcs_India'!X10/'Revised Calcs_India'!$B$10)</f>
-        <v>3410.5916887627463</v>
+        <v>2469.4291883349879</v>
       </c>
       <c r="AC2" s="9">
         <f>$F$2*('Revised Calcs_India'!Y10/'Revised Calcs_India'!$B$10)</f>
-        <v>3548.00018349731</v>
+        <v>2550.2598577817976</v>
       </c>
       <c r="AD2" s="9">
         <f>$F$2*('Revised Calcs_India'!Z10/'Revised Calcs_India'!$B$10)</f>
-        <v>3659.8690656640747</v>
+        <v>2621.0690231843796</v>
       </c>
       <c r="AE2" s="9">
         <f>$F$2*('Revised Calcs_India'!AA10/'Revised Calcs_India'!$B$10)</f>
-        <v>3782.5578231859113</v>
+        <v>2690.2088842305866</v>
       </c>
       <c r="AF2" s="9">
         <f>$F$2*('Revised Calcs_India'!AB10/'Revised Calcs_India'!$B$10)</f>
-        <v>3899.1166254314926</v>
+        <v>2757.8043548518467</v>
       </c>
       <c r="AG2" s="9">
         <f>$F$2*('Revised Calcs_India'!AC10/'Revised Calcs_India'!$B$10)</f>
-        <v>4009.4109944057273</v>
+        <v>2822.4529922725669</v>
       </c>
       <c r="AH2" s="9">
         <f>$F$2*('Revised Calcs_India'!AD10/'Revised Calcs_India'!$B$10)</f>
-        <v>4134.9237898244855</v>
+        <v>2885.199531191975</v>
       </c>
       <c r="AI2" s="9">
         <f>$F$2*('Revised Calcs_India'!AE10/'Revised Calcs_India'!$B$10)</f>
-        <v>4245.0164418060831</v>
+        <v>2946.7650656687774</v>
       </c>
       <c r="AJ2" s="9">
         <f>$F$2*('Revised Calcs_India'!AF10/'Revised Calcs_India'!$B$10)</f>
-        <v>4362.0739332834619</v>
+        <v>3007.0757829253107</v>
       </c>
       <c r="AK2" s="9">
         <f>$F$2*('Revised Calcs_India'!AG10/'Revised Calcs_India'!$B$10)</f>
-        <v>4478.9072947690211</v>
+        <v>3064.9733901428658</v>
       </c>
     </row>
   </sheetData>
@@ -3237,26 +3274,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.265625" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
     <col min="8" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="37" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="37" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3369,7 +3406,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -3390,127 +3427,127 @@
       </c>
       <c r="G2" s="9">
         <f>FORECAST('DRC-PADRC'!G1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!G2</f>
-        <v>6947.3701671700364</v>
+        <v>6968.3589057911595</v>
       </c>
       <c r="H2" s="9">
         <f>FORECAST('DRC-PADRC'!H1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!H2</f>
-        <v>13811.251912388485</v>
+        <v>13853.082256585389</v>
       </c>
       <c r="I2" s="9">
         <f>FORECAST('DRC-PADRC'!I1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!I2</f>
-        <v>20688.189229630403</v>
+        <v>20753.868403380253</v>
       </c>
       <c r="J2" s="9">
         <f>FORECAST('DRC-PADRC'!J1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!J2</f>
-        <v>27555.573005971026</v>
+        <v>27657.323165982929</v>
       </c>
       <c r="K2" s="9">
         <f>FORECAST('DRC-PADRC'!K1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!K2</f>
-        <v>34425.892885204477</v>
+        <v>34564.048402426663</v>
       </c>
       <c r="L2" s="9">
         <f>FORECAST('DRC-PADRC'!L1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!L2</f>
-        <v>41297.535131389668</v>
+        <v>41476.389087878757</v>
       </c>
       <c r="M2" s="9">
         <f>FORECAST('DRC-PADRC'!M1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!M2</f>
-        <v>48170.494141276795</v>
+        <v>48390.416111405139</v>
       </c>
       <c r="N2" s="9">
         <f>FORECAST('DRC-PADRC'!N1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!N2</f>
-        <v>55043.201004923125</v>
+        <v>55300.917155321629</v>
       </c>
       <c r="O2" s="9">
         <f>FORECAST('DRC-PADRC'!O1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!O2</f>
-        <v>61882.523706287982</v>
+        <v>62195.962939176716</v>
       </c>
       <c r="P2" s="9">
         <f>FORECAST('DRC-PADRC'!P1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!P2</f>
-        <v>68721.482196416138</v>
+        <v>69090.174070853609</v>
       </c>
       <c r="Q2" s="9">
         <f>FORECAST('DRC-PADRC'!Q1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Q2</f>
-        <v>75559.717867320665</v>
+        <v>75984.83375710246</v>
       </c>
       <c r="R2" s="9">
         <f>FORECAST('DRC-PADRC'!R1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!R2</f>
-        <v>82398.3401624611</v>
+        <v>82860.216952569346</v>
       </c>
       <c r="S2" s="9">
         <f>FORECAST('DRC-PADRC'!S1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!S2</f>
-        <v>89236.928838102744</v>
+        <v>89734.078469235188</v>
       </c>
       <c r="T2" s="9">
         <f>FORECAST('DRC-PADRC'!T1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!T2</f>
-        <v>96063.78991192246</v>
+        <v>96606.225258296865</v>
       </c>
       <c r="U2" s="9">
         <f>FORECAST('DRC-PADRC'!U1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!U2</f>
-        <v>102890.18031275934</v>
+        <v>103478.60484150347</v>
       </c>
       <c r="V2" s="9">
         <f>FORECAST('DRC-PADRC'!V1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!V2</f>
-        <v>109716.40821935216</v>
+        <v>110352.87516739944</v>
       </c>
       <c r="W2" s="9">
         <f>FORECAST('DRC-PADRC'!W1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!W2</f>
-        <v>116543.06757617924</v>
+        <v>117229.83114282115</v>
       </c>
       <c r="X2" s="9">
         <f>FORECAST('DRC-PADRC'!X1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!X2</f>
-        <v>123367.97871907012</v>
+        <v>124107.84888666001</v>
       </c>
       <c r="Y2" s="9">
         <f>FORECAST('DRC-PADRC'!Y1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Y2</f>
-        <v>130193.27088294709</v>
+        <v>130982.9481868282</v>
       </c>
       <c r="Z2" s="9">
         <f>FORECAST('DRC-PADRC'!Z1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!Z2</f>
-        <v>137019.3250887944</v>
+        <v>137857.62164404648</v>
       </c>
       <c r="AA2" s="9">
         <f>FORECAST('DRC-PADRC'!AA1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AA2</f>
-        <v>143843.64228720695</v>
+        <v>144732.69255468479</v>
       </c>
       <c r="AB2" s="9">
         <f>FORECAST('DRC-PADRC'!AB1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AB2</f>
-        <v>150667.21985664652</v>
+        <v>151608.38235707427</v>
       </c>
       <c r="AC2" s="9">
         <f>FORECAST('DRC-PADRC'!AC1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AC2</f>
-        <v>157491.43059331295</v>
+        <v>158489.17091902849</v>
       </c>
       <c r="AD2" s="9">
         <f>FORECAST('DRC-PADRC'!AD1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AD2</f>
-        <v>164341.18094254722</v>
+        <v>165379.98098502689</v>
       </c>
       <c r="AE2" s="9">
         <f>FORECAST('DRC-PADRC'!AE1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AE2</f>
-        <v>171180.11141642637</v>
+        <v>172272.46035538171</v>
       </c>
       <c r="AF2" s="9">
         <f>FORECAST('DRC-PADRC'!AF1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AF2</f>
-        <v>178025.17184558182</v>
+        <v>179166.48411616147</v>
       </c>
       <c r="AG2" s="9">
         <f>FORECAST('DRC-PADRC'!AG1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AG2</f>
-        <v>184876.49670800858</v>
+        <v>186063.45471014176</v>
       </c>
       <c r="AH2" s="9">
         <f>FORECAST('DRC-PADRC'!AH1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AH2</f>
-        <v>191712.60314399085</v>
+        <v>192962.32740262334</v>
       </c>
       <c r="AI2" s="9">
         <f>FORECAST('DRC-PADRC'!AI1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AI2</f>
-        <v>198564.12972341027</v>
+        <v>199862.38109954755</v>
       </c>
       <c r="AJ2" s="9">
         <f>FORECAST('DRC-PADRC'!AJ1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AJ2</f>
-        <v>205408.6914633339</v>
+        <v>206763.68961369205</v>
       </c>
       <c r="AK2" s="9">
         <f>FORECAST('DRC-PADRC'!AK1,'Revised Calcs_India'!$B$3:$C$3,'Revised Calcs_India'!$B$2:$C$2)-'DRC-BDRC'!AK2</f>
-        <v>212253.47733324935</v>
+        <v>213667.41123787549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>